<commit_message>
added std dev check
</commit_message>
<xml_diff>
--- a/BMI report/Report files/Classification success.xlsx
+++ b/BMI report/Report files/Classification success.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nabee\Desktop\bmi-lekker-meid\BMI report\Report files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA6D3E2E-9F50-4007-9CCA-D2E6E2F055C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C88D4CB8-5232-4CD3-997C-7F0E2A59705E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{60DD41AC-037E-49BB-88B9-F74C7EC24C57}"/>
   </bookViews>
@@ -124,12 +124,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -530,7 +531,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -646,7 +647,7 @@
         <v>3</v>
       </c>
       <c r="B10">
-        <v>17.8</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="C10">
         <v>99.53</v>
@@ -660,12 +661,12 @@
         <v>4</v>
       </c>
       <c r="B11">
-        <v>36.840000000000003</v>
+        <v>33.06</v>
       </c>
       <c r="C11">
         <v>99.29</v>
       </c>
-      <c r="D11">
+      <c r="D11" s="3">
         <v>11.4953</v>
       </c>
     </row>
@@ -674,12 +675,12 @@
         <v>5</v>
       </c>
       <c r="B12">
-        <v>34.92</v>
+        <v>34.69</v>
       </c>
       <c r="C12">
         <v>99.23</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="3">
         <v>11.592599999999999</v>
       </c>
     </row>
@@ -693,7 +694,7 @@
       <c r="C13">
         <v>99.43</v>
       </c>
-      <c r="D13">
+      <c r="D13" s="3">
         <v>11.4909</v>
       </c>
     </row>

</xml_diff>